<commit_message>
Commit in Personal Folder: added Paper of User Views
</commit_message>
<xml_diff>
--- a/Docs/Lukas/workDoc.xlsx
+++ b/Docs/Lukas/workDoc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Work Documentation</t>
   </si>
@@ -45,13 +45,37 @@
   </si>
   <si>
     <t>user description</t>
+  </si>
+  <si>
+    <t>Beschreibung aller in Frage kommenden Nutzer der Anwendung</t>
+  </si>
+  <si>
+    <t>user views</t>
+  </si>
+  <si>
+    <t>Beschreibung von notwendigen Ansichten und damit verbundene Use Cases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,14 +86,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -96,11 +112,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -415,49 +432,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E8"/>
+  <dimension ref="C3:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.85546875" customWidth="1"/>
-    <col min="4" max="4" width="159.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="1" max="2" width="11.42578125" style="2"/>
+    <col min="3" max="3" width="38.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="159.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="4">
         <v>43011</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made slight changes to the document of the user views
</commit_message>
<xml_diff>
--- a/Docs/Lukas/workDoc.xlsx
+++ b/Docs/Lukas/workDoc.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Work Documentation</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Beschreibung von notwendigen Ansichten und damit verbundene Use Cases</t>
+  </si>
+  <si>
+    <t>user view review</t>
+  </si>
+  <si>
+    <t>kleine Nachbesserungen</t>
   </si>
 </sst>
 </file>
@@ -112,12 +118,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -432,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E9"/>
+  <dimension ref="C3:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,6 +488,9 @@
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E8" s="4">
+        <v>43013</v>
+      </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
@@ -488,6 +498,20 @@
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="E9" s="4">
+        <v>43013</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4">
+        <v>43026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>